<commit_message>
fix excel number formatting issue(!)
</commit_message>
<xml_diff>
--- a/zs/0612/valid_entities_0612_prompt1.xlsx
+++ b/zs/0612/valid_entities_0612_prompt1.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Working\hp-extractor\zs\0612\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4308D68E-CFD3-4BEB-B770-0E5324239BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F808D7B1-3A9D-48DF-AADE-7C183FE2B62B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6337" yWindow="240" windowWidth="21600" windowHeight="10905" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2573" yWindow="2160" windowWidth="14992" windowHeight="14040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="entities_0312_prompt1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -7863,9 +7863,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mmm/yy"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -7945,7 +7942,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7966,10 +7963,12 @@
       <alignment horizontal="left" textRotation="45" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8376,13 +8375,13 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S13" sqref="S13"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="2" max="2" width="18.53125" customWidth="1"/>
     <col min="3" max="3" width="16.1328125" customWidth="1"/>
     <col min="4" max="7" width="4.3984375" style="1" customWidth="1"/>
     <col min="8" max="9" width="15.73046875" customWidth="1"/>
@@ -8646,7 +8645,7 @@
       <c r="A20">
         <v>59826</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" t="s">
         <v>27</v>
       </c>
       <c r="C20" t="s">
@@ -8657,7 +8656,7 @@
       <c r="A21">
         <v>59826</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="11">
         <v>46419</v>
       </c>
       <c r="C21" t="s">
@@ -8668,7 +8667,7 @@
       <c r="A22">
         <v>59826</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="11">
         <v>42979</v>
       </c>
       <c r="C22" t="s">
@@ -8690,7 +8689,7 @@
       <c r="A24">
         <v>59826</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="8">
         <v>0.36</v>
       </c>
       <c r="C24" t="s">
@@ -8701,7 +8700,7 @@
       <c r="A25">
         <v>59826</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="8">
         <v>0.13</v>
       </c>
       <c r="C25" t="s">
@@ -8811,7 +8810,7 @@
       <c r="A35">
         <v>58605</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="11">
         <v>31868</v>
       </c>
       <c r="C35" t="s">
@@ -8822,7 +8821,7 @@
       <c r="A36">
         <v>58605</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="11">
         <v>32143</v>
       </c>
       <c r="C36" t="s">
@@ -8921,7 +8920,7 @@
       <c r="A45">
         <v>58605</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" t="s">
         <v>38</v>
       </c>
       <c r="C45" t="s">
@@ -8932,7 +8931,7 @@
       <c r="A46">
         <v>58605</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" t="s">
         <v>39</v>
       </c>
       <c r="C46" t="s">
@@ -9075,7 +9074,7 @@
       <c r="A59">
         <v>58605</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="8">
         <v>0.34</v>
       </c>
       <c r="C59" t="s">
@@ -9108,7 +9107,7 @@
       <c r="A62">
         <v>58605</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="8">
         <v>0.09</v>
       </c>
       <c r="C62" t="s">
@@ -9119,7 +9118,7 @@
       <c r="A63">
         <v>58605</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="11">
         <v>20180</v>
       </c>
       <c r="C63" t="s">
@@ -9130,7 +9129,7 @@
       <c r="A64">
         <v>58605</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="8">
         <v>0.03</v>
       </c>
       <c r="C64" t="s">
@@ -9141,7 +9140,7 @@
       <c r="A65">
         <v>58605</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="11">
         <v>46753</v>
       </c>
       <c r="C65" t="s">
@@ -9152,7 +9151,7 @@
       <c r="A66">
         <v>58605</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="8">
         <v>0.02</v>
       </c>
       <c r="C66" t="s">
@@ -9163,7 +9162,7 @@
       <c r="A67">
         <v>58605</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="11">
         <v>13150</v>
       </c>
       <c r="C67" t="s">
@@ -9196,7 +9195,7 @@
       <c r="A70">
         <v>58605</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="11">
         <v>42614</v>
       </c>
       <c r="C70" t="s">
@@ -9207,7 +9206,7 @@
       <c r="A71">
         <v>58605</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="11">
         <v>46143</v>
       </c>
       <c r="C71" t="s">
@@ -9416,7 +9415,7 @@
       <c r="A90">
         <v>59830</v>
       </c>
-      <c r="B90" s="9" t="s">
+      <c r="B90" t="s">
         <v>66</v>
       </c>
       <c r="C90" t="s">
@@ -9427,7 +9426,7 @@
       <c r="A91">
         <v>59830</v>
       </c>
-      <c r="B91" s="9" t="s">
+      <c r="B91" t="s">
         <v>67</v>
       </c>
       <c r="C91" t="s">
@@ -9592,7 +9591,7 @@
       <c r="A106">
         <v>59830</v>
       </c>
-      <c r="B106" s="10">
+      <c r="B106">
         <v>32</v>
       </c>
       <c r="C106" t="s">
@@ -9614,7 +9613,7 @@
       <c r="A108">
         <v>59830</v>
       </c>
-      <c r="B108">
+      <c r="B108" s="8">
         <v>0.44</v>
       </c>
       <c r="C108" t="s">
@@ -9625,7 +9624,7 @@
       <c r="A109">
         <v>59830</v>
       </c>
-      <c r="B109">
+      <c r="B109" s="8">
         <v>0.47</v>
       </c>
       <c r="C109" t="s">
@@ -9636,7 +9635,7 @@
       <c r="A110">
         <v>59830</v>
       </c>
-      <c r="B110">
+      <c r="B110" s="8">
         <v>0.45</v>
       </c>
       <c r="C110" t="s">
@@ -9713,7 +9712,7 @@
       <c r="A117">
         <v>59699</v>
       </c>
-      <c r="B117" s="9" t="s">
+      <c r="B117" t="s">
         <v>79</v>
       </c>
       <c r="C117" t="s">
@@ -9845,7 +9844,7 @@
       <c r="A129">
         <v>59699</v>
       </c>
-      <c r="B129">
+      <c r="B129" s="8">
         <v>0.97</v>
       </c>
       <c r="C129" t="s">
@@ -9856,7 +9855,7 @@
       <c r="A130">
         <v>59699</v>
       </c>
-      <c r="B130">
+      <c r="B130" s="8">
         <v>0.59</v>
       </c>
       <c r="C130" t="s">
@@ -9955,7 +9954,7 @@
       <c r="A139">
         <v>59904</v>
       </c>
-      <c r="B139">
+      <c r="B139" s="9">
         <v>0.88100000000000001</v>
       </c>
       <c r="C139" t="s">
@@ -9966,7 +9965,7 @@
       <c r="A140">
         <v>59904</v>
       </c>
-      <c r="B140">
+      <c r="B140" s="9">
         <v>0.82099999999999995</v>
       </c>
       <c r="C140" t="s">
@@ -10153,7 +10152,7 @@
       <c r="A157">
         <v>59578</v>
       </c>
-      <c r="B157">
+      <c r="B157" s="8">
         <v>0.42</v>
       </c>
       <c r="C157" t="s">
@@ -10956,7 +10955,7 @@
       <c r="A230">
         <v>59842</v>
       </c>
-      <c r="B230">
+      <c r="B230" s="10">
         <v>1024</v>
       </c>
       <c r="C230" t="s">
@@ -10967,7 +10966,7 @@
       <c r="A231">
         <v>59842</v>
       </c>
-      <c r="B231">
+      <c r="B231" s="12">
         <v>45778</v>
       </c>
       <c r="C231" t="s">
@@ -10978,7 +10977,7 @@
       <c r="A232">
         <v>59842</v>
       </c>
-      <c r="B232">
+      <c r="B232" s="12">
         <v>45780</v>
       </c>
       <c r="C232" t="s">
@@ -10989,7 +10988,7 @@
       <c r="A233">
         <v>59842</v>
       </c>
-      <c r="B233">
+      <c r="B233" s="12">
         <v>45782</v>
       </c>
       <c r="C233" t="s">
@@ -11572,7 +11571,7 @@
       <c r="A286">
         <v>58455</v>
       </c>
-      <c r="B286">
+      <c r="B286" s="8">
         <v>0</v>
       </c>
       <c r="C286" t="s">
@@ -11583,7 +11582,7 @@
       <c r="A287">
         <v>58455</v>
       </c>
-      <c r="B287">
+      <c r="B287" s="8">
         <v>1</v>
       </c>
       <c r="C287" t="s">
@@ -11660,7 +11659,7 @@
       <c r="A294">
         <v>58455</v>
       </c>
-      <c r="B294" s="9" t="s">
+      <c r="B294" t="s">
         <v>1340</v>
       </c>
       <c r="C294" t="s">
@@ -11924,7 +11923,7 @@
       <c r="A318">
         <v>59836</v>
       </c>
-      <c r="B318" s="9" t="s">
+      <c r="B318" t="s">
         <v>195</v>
       </c>
       <c r="C318" t="s">
@@ -11935,7 +11934,7 @@
       <c r="A319">
         <v>59836</v>
       </c>
-      <c r="B319" s="9" t="s">
+      <c r="B319" t="s">
         <v>196</v>
       </c>
       <c r="C319" t="s">
@@ -12001,7 +12000,7 @@
       <c r="A325">
         <v>59836</v>
       </c>
-      <c r="B325">
+      <c r="B325" s="8">
         <v>0.25</v>
       </c>
       <c r="C325" t="s">
@@ -12507,7 +12506,7 @@
       <c r="A371">
         <v>59858</v>
       </c>
-      <c r="B371">
+      <c r="B371" s="8">
         <v>0.65</v>
       </c>
       <c r="C371" t="s">
@@ -12518,7 +12517,7 @@
       <c r="A372">
         <v>59858</v>
       </c>
-      <c r="B372">
+      <c r="B372" s="8">
         <v>0.05</v>
       </c>
       <c r="C372" t="s">
@@ -12815,7 +12814,7 @@
       <c r="A399">
         <v>56169</v>
       </c>
-      <c r="B399" s="9" t="s">
+      <c r="B399" t="s">
         <v>1401</v>
       </c>
       <c r="C399" t="s">
@@ -13013,7 +13012,7 @@
       <c r="A417">
         <v>59837</v>
       </c>
-      <c r="B417" s="10" t="s">
+      <c r="B417" t="s">
         <v>245</v>
       </c>
       <c r="C417" t="s">
@@ -13035,7 +13034,7 @@
       <c r="A419">
         <v>59837</v>
       </c>
-      <c r="B419" s="10" t="s">
+      <c r="B419" t="s">
         <v>247</v>
       </c>
       <c r="C419" t="s">
@@ -13046,7 +13045,7 @@
       <c r="A420">
         <v>59837</v>
       </c>
-      <c r="B420" s="10" t="s">
+      <c r="B420" t="s">
         <v>248</v>
       </c>
       <c r="C420" t="s">
@@ -13057,7 +13056,7 @@
       <c r="A421">
         <v>59837</v>
       </c>
-      <c r="B421" s="10" t="s">
+      <c r="B421" t="s">
         <v>49</v>
       </c>
       <c r="C421" t="s">
@@ -13299,7 +13298,7 @@
       <c r="A443">
         <v>59837</v>
       </c>
-      <c r="B443">
+      <c r="B443" s="8">
         <v>0.79</v>
       </c>
       <c r="C443" t="s">
@@ -13332,7 +13331,7 @@
       <c r="A446">
         <v>59837</v>
       </c>
-      <c r="B446">
+      <c r="B446" s="8">
         <v>0.04</v>
       </c>
       <c r="C446" t="s">
@@ -13365,7 +13364,7 @@
       <c r="A449">
         <v>59837</v>
       </c>
-      <c r="B449">
+      <c r="B449" s="8">
         <v>0.2</v>
       </c>
       <c r="C449" t="s">
@@ -13387,7 +13386,7 @@
       <c r="A451">
         <v>59837</v>
       </c>
-      <c r="B451">
+      <c r="B451" s="8">
         <v>0.01</v>
       </c>
       <c r="C451" t="s">
@@ -13398,7 +13397,7 @@
       <c r="A452">
         <v>59837</v>
       </c>
-      <c r="B452">
+      <c r="B452" s="8">
         <v>0.67</v>
       </c>
       <c r="C452" t="s">
@@ -13409,7 +13408,7 @@
       <c r="A453">
         <v>59837</v>
       </c>
-      <c r="B453">
+      <c r="B453" s="8">
         <v>0.15</v>
       </c>
       <c r="C453" t="s">
@@ -13574,7 +13573,7 @@
       <c r="A468">
         <v>59823</v>
       </c>
-      <c r="B468" s="9" t="s">
+      <c r="B468" t="s">
         <v>1451</v>
       </c>
       <c r="C468" t="s">
@@ -13783,7 +13782,7 @@
       <c r="A487">
         <v>57733</v>
       </c>
-      <c r="B487" s="9" t="s">
+      <c r="B487" t="s">
         <v>268</v>
       </c>
       <c r="C487" t="s">
@@ -13816,7 +13815,7 @@
       <c r="A490">
         <v>57733</v>
       </c>
-      <c r="B490">
+      <c r="B490" s="8">
         <v>0.44</v>
       </c>
       <c r="C490" t="s">
@@ -14124,7 +14123,7 @@
       <c r="A518">
         <v>59859</v>
       </c>
-      <c r="B518">
+      <c r="B518" s="9">
         <v>0.41699999999999998</v>
       </c>
       <c r="C518" t="s">
@@ -14146,7 +14145,7 @@
       <c r="A520">
         <v>59859</v>
       </c>
-      <c r="B520">
+      <c r="B520" s="8">
         <v>1</v>
       </c>
       <c r="C520" t="s">
@@ -14179,7 +14178,7 @@
       <c r="A523">
         <v>59859</v>
       </c>
-      <c r="B523">
+      <c r="B523" s="9">
         <v>0.80700000000000005</v>
       </c>
       <c r="C523" t="s">
@@ -14212,7 +14211,7 @@
       <c r="A526">
         <v>59859</v>
       </c>
-      <c r="B526">
+      <c r="B526" s="9">
         <v>2.7E-2</v>
       </c>
       <c r="C526" t="s">
@@ -14223,7 +14222,7 @@
       <c r="A527">
         <v>59859</v>
       </c>
-      <c r="B527">
+      <c r="B527" s="9">
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="C527" t="s">
@@ -14366,7 +14365,7 @@
       <c r="A540">
         <v>56156</v>
       </c>
-      <c r="B540" s="9" t="s">
+      <c r="B540" t="s">
         <v>281</v>
       </c>
       <c r="C540" t="s">
@@ -14377,7 +14376,7 @@
       <c r="A541">
         <v>56156</v>
       </c>
-      <c r="B541" s="9" t="s">
+      <c r="B541" t="s">
         <v>1491</v>
       </c>
       <c r="C541" t="s">
@@ -14388,7 +14387,7 @@
       <c r="A542">
         <v>56156</v>
       </c>
-      <c r="B542" s="9" t="s">
+      <c r="B542" t="s">
         <v>283</v>
       </c>
       <c r="C542" t="s">
@@ -14399,7 +14398,7 @@
       <c r="A543">
         <v>56156</v>
       </c>
-      <c r="B543" s="9" t="s">
+      <c r="B543" t="s">
         <v>285</v>
       </c>
       <c r="C543" t="s">
@@ -14795,7 +14794,7 @@
       <c r="A579">
         <v>56805</v>
       </c>
-      <c r="B579">
+      <c r="B579" s="8">
         <v>0.3</v>
       </c>
       <c r="C579" t="s">
@@ -14806,7 +14805,7 @@
       <c r="A580">
         <v>56805</v>
       </c>
-      <c r="B580">
+      <c r="B580" s="8">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="C580" t="s">
@@ -15620,7 +15619,7 @@
       <c r="A654">
         <v>59886</v>
       </c>
-      <c r="B654">
+      <c r="B654" s="8">
         <v>0.14000000000000001</v>
       </c>
       <c r="C654" t="s">
@@ -15631,7 +15630,7 @@
       <c r="A655">
         <v>59886</v>
       </c>
-      <c r="B655">
+      <c r="B655" s="8">
         <v>0.08</v>
       </c>
       <c r="C655" t="s">
@@ -15642,7 +15641,7 @@
       <c r="A656">
         <v>59886</v>
       </c>
-      <c r="B656">
+      <c r="B656" s="8">
         <v>0.5</v>
       </c>
       <c r="C656" t="s">
@@ -15653,7 +15652,7 @@
       <c r="A657">
         <v>59886</v>
       </c>
-      <c r="B657">
+      <c r="B657" s="8">
         <v>0.33</v>
       </c>
       <c r="C657" t="s">
@@ -16203,7 +16202,7 @@
       <c r="A707">
         <v>59832</v>
       </c>
-      <c r="B707">
+      <c r="B707" s="8">
         <v>0.21</v>
       </c>
       <c r="C707" t="s">
@@ -16225,7 +16224,7 @@
       <c r="A709">
         <v>59832</v>
       </c>
-      <c r="B709">
+      <c r="B709" s="8">
         <v>0.87</v>
       </c>
       <c r="C709" t="s">
@@ -16247,7 +16246,7 @@
       <c r="A711">
         <v>59832</v>
       </c>
-      <c r="B711">
+      <c r="B711" s="8">
         <v>0.09</v>
       </c>
       <c r="C711" t="s">
@@ -16577,7 +16576,7 @@
       <c r="A741">
         <v>60194</v>
       </c>
-      <c r="B741" s="8" t="s">
+      <c r="B741" t="s">
         <v>1584</v>
       </c>
       <c r="C741" t="s">
@@ -16588,7 +16587,7 @@
       <c r="A742">
         <v>60194</v>
       </c>
-      <c r="B742" s="8" t="s">
+      <c r="B742" t="s">
         <v>1586</v>
       </c>
       <c r="C742" t="s">
@@ -16643,7 +16642,7 @@
       <c r="A747">
         <v>60194</v>
       </c>
-      <c r="B747">
+      <c r="B747" s="9">
         <v>0.27100000000000002</v>
       </c>
       <c r="C747" t="s">
@@ -16654,7 +16653,7 @@
       <c r="A748">
         <v>60194</v>
       </c>
-      <c r="B748">
+      <c r="B748" s="9">
         <v>0.373</v>
       </c>
       <c r="C748" t="s">
@@ -16665,7 +16664,7 @@
       <c r="A749">
         <v>60194</v>
       </c>
-      <c r="B749">
+      <c r="B749" s="9">
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="C749" t="s">
@@ -16676,7 +16675,7 @@
       <c r="A750">
         <v>60194</v>
       </c>
-      <c r="B750">
+      <c r="B750" s="9">
         <v>0.10199999999999999</v>
       </c>
       <c r="C750" t="s">
@@ -16687,7 +16686,7 @@
       <c r="A751">
         <v>60194</v>
       </c>
-      <c r="B751">
+      <c r="B751" s="9">
         <v>0.20300000000000001</v>
       </c>
       <c r="C751" t="s">
@@ -16698,7 +16697,7 @@
       <c r="A752">
         <v>60194</v>
       </c>
-      <c r="B752">
+      <c r="B752" s="9">
         <v>0.83099999999999996</v>
       </c>
       <c r="C752" t="s">
@@ -16709,7 +16708,7 @@
       <c r="A753">
         <v>60194</v>
       </c>
-      <c r="B753">
+      <c r="B753" s="9">
         <v>0.16900000000000001</v>
       </c>
       <c r="C753" t="s">
@@ -16720,7 +16719,7 @@
       <c r="A754">
         <v>60194</v>
       </c>
-      <c r="B754">
+      <c r="B754" s="9">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="C754" t="s">
@@ -16731,7 +16730,7 @@
       <c r="A755">
         <v>60194</v>
       </c>
-      <c r="B755">
+      <c r="B755" s="9">
         <v>0.13300000000000001</v>
       </c>
       <c r="C755" t="s">
@@ -16742,7 +16741,7 @@
       <c r="A756">
         <v>60194</v>
       </c>
-      <c r="B756">
+      <c r="B756" s="9">
         <v>0.11899999999999999</v>
       </c>
       <c r="C756" t="s">
@@ -16753,7 +16752,7 @@
       <c r="A757">
         <v>60194</v>
       </c>
-      <c r="B757">
+      <c r="B757" s="9">
         <v>0.36599999999999999</v>
       </c>
       <c r="C757" t="s">
@@ -16764,7 +16763,7 @@
       <c r="A758">
         <v>60194</v>
       </c>
-      <c r="B758">
+      <c r="B758" s="9">
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="C758" t="s">
@@ -16775,7 +16774,7 @@
       <c r="A759">
         <v>60194</v>
       </c>
-      <c r="B759">
+      <c r="B759" s="9">
         <v>0.61</v>
       </c>
       <c r="C759" t="s">
@@ -16786,7 +16785,7 @@
       <c r="A760">
         <v>60194</v>
       </c>
-      <c r="B760">
+      <c r="B760" s="9">
         <v>0.24399999999999999</v>
       </c>
       <c r="C760" t="s">
@@ -16797,7 +16796,7 @@
       <c r="A761">
         <v>60194</v>
       </c>
-      <c r="B761">
+      <c r="B761" s="9">
         <v>0.34200000000000003</v>
       </c>
       <c r="C761" t="s">
@@ -16808,7 +16807,7 @@
       <c r="A762">
         <v>60194</v>
       </c>
-      <c r="B762">
+      <c r="B762" s="9">
         <v>0.22</v>
       </c>
       <c r="C762" t="s">
@@ -16819,7 +16818,7 @@
       <c r="A763">
         <v>60194</v>
       </c>
-      <c r="B763">
+      <c r="B763" s="9">
         <v>0.29299999999999998</v>
       </c>
       <c r="C763" t="s">
@@ -17061,7 +17060,7 @@
       <c r="A785">
         <v>60248</v>
       </c>
-      <c r="B785" s="9" t="s">
+      <c r="B785" t="s">
         <v>1606</v>
       </c>
       <c r="C785" t="s">
@@ -17072,7 +17071,7 @@
       <c r="A786">
         <v>60248</v>
       </c>
-      <c r="B786" s="9" t="s">
+      <c r="B786" t="s">
         <v>1607</v>
       </c>
       <c r="C786" t="s">
@@ -17435,7 +17434,7 @@
       <c r="A819">
         <v>60137</v>
       </c>
-      <c r="B819">
+      <c r="B819" s="8">
         <v>0.8</v>
       </c>
       <c r="C819" t="s">
@@ -17446,7 +17445,7 @@
       <c r="A820">
         <v>60137</v>
       </c>
-      <c r="B820">
+      <c r="B820" s="8">
         <v>0.81</v>
       </c>
       <c r="C820" t="s">
@@ -17457,7 +17456,7 @@
       <c r="A821">
         <v>60137</v>
       </c>
-      <c r="B821">
+      <c r="B821" s="8">
         <v>0.08</v>
       </c>
       <c r="C821" t="s">
@@ -17468,7 +17467,7 @@
       <c r="A822">
         <v>60137</v>
       </c>
-      <c r="B822">
+      <c r="B822" s="8">
         <v>0.27</v>
       </c>
       <c r="C822" t="s">
@@ -17479,7 +17478,7 @@
       <c r="A823">
         <v>60137</v>
       </c>
-      <c r="B823">
+      <c r="B823" s="8">
         <v>0.4</v>
       </c>
       <c r="C823" t="s">
@@ -17952,7 +17951,7 @@
       <c r="A866">
         <v>60321</v>
       </c>
-      <c r="B866" s="8">
+      <c r="B866">
         <v>662</v>
       </c>
       <c r="C866" t="s">
@@ -17963,7 +17962,7 @@
       <c r="A867">
         <v>60321</v>
       </c>
-      <c r="B867" s="8">
+      <c r="B867">
         <v>86</v>
       </c>
       <c r="C867" t="s">
@@ -18282,7 +18281,7 @@
       <c r="A896">
         <v>60365</v>
       </c>
-      <c r="B896">
+      <c r="B896" s="11">
         <v>38412</v>
       </c>
       <c r="C896" t="s">
@@ -18293,7 +18292,7 @@
       <c r="A897">
         <v>60365</v>
       </c>
-      <c r="B897">
+      <c r="B897" s="11">
         <v>39083</v>
       </c>
       <c r="C897" t="s">
@@ -19371,7 +19370,7 @@
       <c r="A995">
         <v>60155</v>
       </c>
-      <c r="B995">
+      <c r="B995" s="8">
         <v>0.49</v>
       </c>
       <c r="C995" t="s">
@@ -19393,7 +19392,7 @@
       <c r="A997">
         <v>60155</v>
       </c>
-      <c r="B997">
+      <c r="B997" s="8">
         <v>0.38</v>
       </c>
       <c r="C997" t="s">
@@ -19415,7 +19414,7 @@
       <c r="A999">
         <v>60155</v>
       </c>
-      <c r="B999">
+      <c r="B999" s="8">
         <v>0.17</v>
       </c>
       <c r="C999" t="s">
@@ -19426,7 +19425,7 @@
       <c r="A1000">
         <v>60155</v>
       </c>
-      <c r="B1000">
+      <c r="B1000" s="8">
         <v>0.06</v>
       </c>
       <c r="C1000" t="s">
@@ -20119,7 +20118,7 @@
       <c r="A1063">
         <v>60186</v>
       </c>
-      <c r="B1063">
+      <c r="B1063" s="11">
         <v>34608</v>
       </c>
       <c r="C1063" t="s">
@@ -20130,7 +20129,7 @@
       <c r="A1064">
         <v>60186</v>
       </c>
-      <c r="B1064">
+      <c r="B1064" s="11">
         <v>34943</v>
       </c>
       <c r="C1064" t="s">
@@ -20933,7 +20932,7 @@
       <c r="A1137">
         <v>60214</v>
       </c>
-      <c r="B1137" s="8" t="s">
+      <c r="B1137" t="s">
         <v>1843</v>
       </c>
       <c r="C1137" t="s">
@@ -21010,7 +21009,7 @@
       <c r="A1144">
         <v>60214</v>
       </c>
-      <c r="B1144" s="8" t="s">
+      <c r="B1144" t="s">
         <v>565</v>
       </c>
       <c r="C1144" t="s">
@@ -22033,7 +22032,7 @@
       <c r="A1237">
         <v>60195</v>
       </c>
-      <c r="B1237" s="8" t="s">
+      <c r="B1237" t="s">
         <v>604</v>
       </c>
       <c r="C1237" t="s">
@@ -22077,7 +22076,7 @@
       <c r="A1241">
         <v>60195</v>
       </c>
-      <c r="B1241" s="8" t="s">
+      <c r="B1241" t="s">
         <v>605</v>
       </c>
       <c r="C1241" t="s">
@@ -22143,7 +22142,7 @@
       <c r="A1247">
         <v>60195</v>
       </c>
-      <c r="B1247">
+      <c r="B1247" s="8">
         <v>0.41</v>
       </c>
       <c r="C1247" t="s">
@@ -22154,7 +22153,7 @@
       <c r="A1248">
         <v>60195</v>
       </c>
-      <c r="B1248">
+      <c r="B1248" s="8">
         <v>0.33</v>
       </c>
       <c r="C1248" t="s">
@@ -22165,7 +22164,7 @@
       <c r="A1249">
         <v>60195</v>
       </c>
-      <c r="B1249">
+      <c r="B1249" s="8">
         <v>0.27</v>
       </c>
       <c r="C1249" t="s">
@@ -22396,7 +22395,7 @@
       <c r="A1270">
         <v>60135</v>
       </c>
-      <c r="B1270" s="8" t="s">
+      <c r="B1270" t="s">
         <v>1933</v>
       </c>
       <c r="C1270" t="s">
@@ -22616,7 +22615,7 @@
       <c r="A1290">
         <v>60291</v>
       </c>
-      <c r="B1290" s="8" t="s">
+      <c r="B1290" t="s">
         <v>1818</v>
       </c>
       <c r="C1290" t="s">
@@ -23232,7 +23231,7 @@
       <c r="A1346">
         <v>60431</v>
       </c>
-      <c r="B1346">
+      <c r="B1346" s="11">
         <v>36069</v>
       </c>
       <c r="C1346" t="s">
@@ -23243,7 +23242,7 @@
       <c r="A1347">
         <v>60431</v>
       </c>
-      <c r="B1347">
+      <c r="B1347" s="11">
         <v>36220</v>
       </c>
       <c r="C1347" t="s">
@@ -23353,7 +23352,7 @@
       <c r="A1357">
         <v>60431</v>
       </c>
-      <c r="B1357" s="9" t="s">
+      <c r="B1357" t="s">
         <v>658</v>
       </c>
       <c r="C1357" t="s">
@@ -23408,7 +23407,7 @@
       <c r="A1362">
         <v>60431</v>
       </c>
-      <c r="B1362">
+      <c r="B1362" s="8">
         <v>0.34</v>
       </c>
       <c r="C1362" t="s">
@@ -23419,7 +23418,7 @@
       <c r="A1363">
         <v>60431</v>
       </c>
-      <c r="B1363">
+      <c r="B1363" s="8">
         <v>0.2</v>
       </c>
       <c r="C1363" t="s">
@@ -23749,7 +23748,7 @@
       <c r="A1393">
         <v>60177</v>
       </c>
-      <c r="B1393" s="9" t="s">
+      <c r="B1393" t="s">
         <v>681</v>
       </c>
       <c r="C1393" t="s">
@@ -23991,7 +23990,7 @@
       <c r="A1415">
         <v>60522</v>
       </c>
-      <c r="B1415" s="10" t="s">
+      <c r="B1415" t="s">
         <v>695</v>
       </c>
       <c r="C1415" t="s">
@@ -24002,7 +24001,7 @@
       <c r="A1416">
         <v>60522</v>
       </c>
-      <c r="B1416" s="10" t="s">
+      <c r="B1416" t="s">
         <v>2003</v>
       </c>
       <c r="C1416" t="s">
@@ -24013,7 +24012,7 @@
       <c r="A1417">
         <v>60522</v>
       </c>
-      <c r="B1417" s="10">
+      <c r="B1417">
         <v>1766</v>
       </c>
       <c r="C1417" t="s">
@@ -24024,7 +24023,7 @@
       <c r="A1418">
         <v>60522</v>
       </c>
-      <c r="B1418" s="10" t="s">
+      <c r="B1418" t="s">
         <v>44</v>
       </c>
       <c r="C1418" t="s">
@@ -24431,7 +24430,7 @@
       <c r="A1455">
         <v>60223</v>
       </c>
-      <c r="B1455">
+      <c r="B1455" s="11">
         <v>36434</v>
       </c>
       <c r="C1455" t="s">
@@ -24442,7 +24441,7 @@
       <c r="A1456">
         <v>60223</v>
       </c>
-      <c r="B1456">
+      <c r="B1456" s="11">
         <v>36831</v>
       </c>
       <c r="C1456" t="s">
@@ -24761,7 +24760,7 @@
       <c r="A1485">
         <v>60200</v>
       </c>
-      <c r="B1485">
+      <c r="B1485" s="11">
         <v>38169</v>
       </c>
       <c r="C1485" t="s">
@@ -24772,7 +24771,7 @@
       <c r="A1486">
         <v>60200</v>
       </c>
-      <c r="B1486">
+      <c r="B1486" s="11">
         <v>38565</v>
       </c>
       <c r="C1486" t="s">
@@ -24904,7 +24903,7 @@
       <c r="A1498">
         <v>60200</v>
       </c>
-      <c r="B1498" s="9" t="s">
+      <c r="B1498" t="s">
         <v>739</v>
       </c>
       <c r="C1498" t="s">
@@ -24915,7 +24914,7 @@
       <c r="A1499">
         <v>60200</v>
       </c>
-      <c r="B1499" s="9" t="s">
+      <c r="B1499" t="s">
         <v>2045</v>
       </c>
       <c r="C1499" t="s">
@@ -24937,7 +24936,7 @@
       <c r="A1501">
         <v>60200</v>
       </c>
-      <c r="B1501" s="9" t="s">
+      <c r="B1501" t="s">
         <v>2047</v>
       </c>
       <c r="C1501" t="s">
@@ -25289,7 +25288,7 @@
       <c r="A1533">
         <v>60178</v>
       </c>
-      <c r="B1533" s="9" t="s">
+      <c r="B1533" t="s">
         <v>1823</v>
       </c>
       <c r="C1533" t="s">
@@ -25311,7 +25310,7 @@
       <c r="A1535">
         <v>60178</v>
       </c>
-      <c r="B1535" s="9" t="s">
+      <c r="B1535" t="s">
         <v>2066</v>
       </c>
       <c r="C1535" t="s">
@@ -26158,7 +26157,7 @@
       <c r="A1612">
         <v>60415</v>
       </c>
-      <c r="B1612">
+      <c r="B1612" s="8">
         <v>0.54</v>
       </c>
       <c r="C1612" t="s">
@@ -26356,7 +26355,7 @@
       <c r="A1630">
         <v>60412</v>
       </c>
-      <c r="B1630">
+      <c r="B1630" s="9">
         <v>0.158</v>
       </c>
       <c r="C1630" t="s">
@@ -26367,7 +26366,7 @@
       <c r="A1631">
         <v>60412</v>
       </c>
-      <c r="B1631">
+      <c r="B1631" s="9">
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="C1631" t="s">
@@ -26400,7 +26399,7 @@
       <c r="A1634">
         <v>60412</v>
       </c>
-      <c r="B1634">
+      <c r="B1634" s="9">
         <v>0.32300000000000001</v>
       </c>
       <c r="C1634" t="s">
@@ -26411,7 +26410,7 @@
       <c r="A1635">
         <v>60412</v>
       </c>
-      <c r="B1635">
+      <c r="B1635" s="8">
         <v>0.5</v>
       </c>
       <c r="C1635" t="s">
@@ -26422,7 +26421,7 @@
       <c r="A1636">
         <v>60412</v>
       </c>
-      <c r="B1636">
+      <c r="B1636" s="8">
         <v>0.21</v>
       </c>
       <c r="C1636" t="s">
@@ -26433,7 +26432,7 @@
       <c r="A1637">
         <v>60412</v>
       </c>
-      <c r="B1637">
+      <c r="B1637" s="9">
         <v>0.28599999999999998</v>
       </c>
       <c r="C1637" t="s">
@@ -26906,7 +26905,7 @@
       <c r="A1680">
         <v>60487</v>
       </c>
-      <c r="B1680" s="10" t="s">
+      <c r="B1680" t="s">
         <v>807</v>
       </c>
       <c r="C1680" t="s">
@@ -27071,7 +27070,7 @@
       <c r="A1695">
         <v>60487</v>
       </c>
-      <c r="B1695" s="9" t="s">
+      <c r="B1695" t="s">
         <v>673</v>
       </c>
       <c r="C1695" t="s">
@@ -27159,7 +27158,7 @@
       <c r="A1703">
         <v>60487</v>
       </c>
-      <c r="B1703">
+      <c r="B1703" s="8">
         <v>0.96</v>
       </c>
       <c r="C1703" t="s">
@@ -27170,7 +27169,7 @@
       <c r="A1704">
         <v>60487</v>
       </c>
-      <c r="B1704">
+      <c r="B1704" s="8">
         <v>0.36</v>
       </c>
       <c r="C1704" t="s">
@@ -27401,7 +27400,7 @@
       <c r="A1725">
         <v>60566</v>
       </c>
-      <c r="B1725">
+      <c r="B1725" s="8">
         <v>0.65</v>
       </c>
       <c r="C1725" t="s">
@@ -27489,7 +27488,7 @@
       <c r="A1733">
         <v>60553</v>
       </c>
-      <c r="B1733" s="10" t="s">
+      <c r="B1733" t="s">
         <v>2158</v>
       </c>
       <c r="C1733" t="s">
@@ -27753,7 +27752,7 @@
       <c r="A1757">
         <v>60511</v>
       </c>
-      <c r="B1757">
+      <c r="B1757" s="8">
         <v>0.21</v>
       </c>
       <c r="C1757" t="s">
@@ -27786,7 +27785,7 @@
       <c r="A1760">
         <v>60511</v>
       </c>
-      <c r="B1760">
+      <c r="B1760" s="8">
         <v>0.44</v>
       </c>
       <c r="C1760" t="s">
@@ -27797,7 +27796,7 @@
       <c r="A1761">
         <v>60511</v>
       </c>
-      <c r="B1761">
+      <c r="B1761" s="13">
         <v>7.6388888888888895E-2</v>
       </c>
       <c r="C1761" t="s">
@@ -28204,7 +28203,7 @@
       <c r="A1798">
         <v>60565</v>
       </c>
-      <c r="B1798" s="10" t="s">
+      <c r="B1798" t="s">
         <v>2194</v>
       </c>
       <c r="C1798" t="s">
@@ -28226,7 +28225,7 @@
       <c r="A1800">
         <v>60565</v>
       </c>
-      <c r="B1800" s="9" t="s">
+      <c r="B1800" t="s">
         <v>2090</v>
       </c>
       <c r="C1800" t="s">
@@ -28479,7 +28478,7 @@
       <c r="A1823">
         <v>60516</v>
       </c>
-      <c r="B1823" s="8" t="s">
+      <c r="B1823" t="s">
         <v>2214</v>
       </c>
       <c r="C1823" t="s">
@@ -28490,7 +28489,7 @@
       <c r="A1824">
         <v>60460</v>
       </c>
-      <c r="B1824" s="8" t="s">
+      <c r="B1824" t="s">
         <v>2216</v>
       </c>
       <c r="C1824" t="s">
@@ -28501,7 +28500,7 @@
       <c r="A1825">
         <v>60460</v>
       </c>
-      <c r="B1825" s="11" t="s">
+      <c r="B1825" t="s">
         <v>2217</v>
       </c>
       <c r="C1825" t="s">
@@ -28523,7 +28522,7 @@
       <c r="A1827">
         <v>60460</v>
       </c>
-      <c r="B1827" s="11" t="s">
+      <c r="B1827" t="s">
         <v>2219</v>
       </c>
       <c r="C1827" t="s">
@@ -28556,7 +28555,7 @@
       <c r="A1830">
         <v>60460</v>
       </c>
-      <c r="B1830" s="9" t="s">
+      <c r="B1830" t="s">
         <v>867</v>
       </c>
       <c r="C1830" t="s">
@@ -28809,7 +28808,7 @@
       <c r="A1853">
         <v>60460</v>
       </c>
-      <c r="B1853">
+      <c r="B1853" s="9">
         <v>3.73E-2</v>
       </c>
       <c r="C1853" t="s">
@@ -29326,7 +29325,7 @@
       <c r="A1900">
         <v>59954</v>
       </c>
-      <c r="B1900" s="10" t="s">
+      <c r="B1900" t="s">
         <v>889</v>
       </c>
       <c r="C1900" t="s">
@@ -29568,7 +29567,7 @@
       <c r="A1922">
         <v>59954</v>
       </c>
-      <c r="B1922" s="9" t="s">
+      <c r="B1922" t="s">
         <v>900</v>
       </c>
       <c r="C1922" t="s">
@@ -29667,7 +29666,7 @@
       <c r="A1931">
         <v>59037</v>
       </c>
-      <c r="B1931" s="10" t="s">
+      <c r="B1931" t="s">
         <v>909</v>
       </c>
       <c r="C1931" t="s">
@@ -29777,7 +29776,7 @@
       <c r="A1941">
         <v>59037</v>
       </c>
-      <c r="B1941" s="11" t="s">
+      <c r="B1941" t="s">
         <v>31</v>
       </c>
       <c r="C1941" t="s">
@@ -29788,7 +29787,7 @@
       <c r="A1942">
         <v>59037</v>
       </c>
-      <c r="B1942" s="10">
+      <c r="B1942" s="8">
         <v>0.99</v>
       </c>
       <c r="C1942" t="s">
@@ -29865,7 +29864,7 @@
       <c r="A1949">
         <v>57824</v>
       </c>
-      <c r="B1949" s="8" t="s">
+      <c r="B1949" t="s">
         <v>2302</v>
       </c>
       <c r="C1949" t="s">
@@ -29887,7 +29886,7 @@
       <c r="A1951">
         <v>57824</v>
       </c>
-      <c r="B1951" s="10" t="s">
+      <c r="B1951" t="s">
         <v>2305</v>
       </c>
       <c r="C1951" t="s">
@@ -29964,7 +29963,7 @@
       <c r="A1958">
         <v>57824</v>
       </c>
-      <c r="B1958" s="8" t="s">
+      <c r="B1958" t="s">
         <v>921</v>
       </c>
       <c r="C1958" t="s">
@@ -29975,7 +29974,7 @@
       <c r="A1959">
         <v>57824</v>
       </c>
-      <c r="B1959" s="11" t="s">
+      <c r="B1959" t="s">
         <v>2313</v>
       </c>
       <c r="C1959" t="s">
@@ -29997,7 +29996,7 @@
       <c r="A1961">
         <v>57824</v>
       </c>
-      <c r="B1961" s="10" t="s">
+      <c r="B1961" t="s">
         <v>2314</v>
       </c>
       <c r="C1961" t="s">
@@ -30008,7 +30007,7 @@
       <c r="A1962">
         <v>57824</v>
       </c>
-      <c r="B1962" s="10" t="s">
+      <c r="B1962" t="s">
         <v>2316</v>
       </c>
       <c r="C1962" t="s">
@@ -30031,6 +30030,7 @@
         <v>57824</v>
       </c>
       <c r="B1964" t="e">
+        <f>-non-encoding region</f>
         <v>#NAME?</v>
       </c>
       <c r="C1964" t="s">
@@ -30316,7 +30316,7 @@
       <c r="A1990">
         <v>59194</v>
       </c>
-      <c r="B1990">
+      <c r="B1990" s="9">
         <v>0.122</v>
       </c>
       <c r="C1990" t="s">
@@ -30932,7 +30932,7 @@
       <c r="A2046">
         <v>60043</v>
       </c>
-      <c r="B2046" s="10">
+      <c r="B2046">
         <v>41</v>
       </c>
       <c r="C2046" t="s">
@@ -30943,7 +30943,7 @@
       <c r="A2047">
         <v>60043</v>
       </c>
-      <c r="B2047">
+      <c r="B2047" s="8">
         <v>0.56000000000000005</v>
       </c>
       <c r="C2047" t="s">
@@ -30954,7 +30954,7 @@
       <c r="A2048">
         <v>60043</v>
       </c>
-      <c r="B2048">
+      <c r="B2048" s="8">
         <v>0.8</v>
       </c>
       <c r="C2048" t="s">
@@ -30965,7 +30965,7 @@
       <c r="A2049">
         <v>60043</v>
       </c>
-      <c r="B2049">
+      <c r="B2049" s="8">
         <v>0.05</v>
       </c>
       <c r="C2049" t="s">
@@ -31295,7 +31295,7 @@
       <c r="A2079">
         <v>58382</v>
       </c>
-      <c r="B2079">
+      <c r="B2079" s="11">
         <v>39722</v>
       </c>
       <c r="C2079" t="s">
@@ -31306,7 +31306,7 @@
       <c r="A2080">
         <v>58382</v>
       </c>
-      <c r="B2080">
+      <c r="B2080" s="11">
         <v>39965</v>
       </c>
       <c r="C2080" t="s">
@@ -31317,7 +31317,7 @@
       <c r="A2081">
         <v>58382</v>
       </c>
-      <c r="B2081" s="9">
+      <c r="B2081" s="10">
         <v>2013</v>
       </c>
       <c r="C2081" t="s">
@@ -31339,7 +31339,7 @@
       <c r="A2083">
         <v>58382</v>
       </c>
-      <c r="B2083">
+      <c r="B2083" s="10">
         <v>1183</v>
       </c>
       <c r="C2083" t="s">
@@ -32043,7 +32043,7 @@
       <c r="A2147">
         <v>59229</v>
       </c>
-      <c r="B2147">
+      <c r="B2147" s="11">
         <v>37104</v>
       </c>
       <c r="C2147" t="s">
@@ -32175,7 +32175,7 @@
       <c r="A2159">
         <v>59229</v>
       </c>
-      <c r="B2159">
+      <c r="B2159" s="9">
         <v>0.995</v>
       </c>
       <c r="C2159" t="s">
@@ -32659,7 +32659,7 @@
       <c r="A2203">
         <v>58774</v>
       </c>
-      <c r="B2203" s="10">
+      <c r="B2203">
         <v>394</v>
       </c>
       <c r="C2203" t="s">
@@ -33055,7 +33055,7 @@
       <c r="A2239">
         <v>60097</v>
       </c>
-      <c r="B2239">
+      <c r="B2239" s="11">
         <v>33239</v>
       </c>
       <c r="C2239" t="s">
@@ -33066,7 +33066,7 @@
       <c r="A2240">
         <v>60097</v>
       </c>
-      <c r="B2240">
+      <c r="B2240" s="11">
         <v>34669</v>
       </c>
       <c r="C2240" t="s">
@@ -33077,7 +33077,7 @@
       <c r="A2241">
         <v>60097</v>
       </c>
-      <c r="B2241">
+      <c r="B2241" s="10">
         <v>3143</v>
       </c>
       <c r="C2241" t="s">
@@ -33099,7 +33099,7 @@
       <c r="A2243">
         <v>60097</v>
       </c>
-      <c r="B2243">
+      <c r="B2243" s="9">
         <v>8.8999999999999996E-2</v>
       </c>
       <c r="C2243" t="s">
@@ -33121,7 +33121,7 @@
       <c r="A2245">
         <v>60097</v>
       </c>
-      <c r="B2245">
+      <c r="B2245" s="9">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C2245" t="s">
@@ -33154,7 +33154,7 @@
       <c r="A2248">
         <v>60097</v>
       </c>
-      <c r="B2248">
+      <c r="B2248" s="9">
         <v>0.748</v>
       </c>
       <c r="C2248" t="s">
@@ -33231,7 +33231,7 @@
       <c r="A2255">
         <v>60097</v>
       </c>
-      <c r="B2255">
+      <c r="B2255" s="8">
         <v>0.22</v>
       </c>
       <c r="C2255" t="s">
@@ -33594,7 +33594,7 @@
       <c r="A2288">
         <v>57815</v>
       </c>
-      <c r="B2288">
+      <c r="B2288" s="9">
         <v>0.44400000000000001</v>
       </c>
       <c r="C2288" t="s">
@@ -33605,7 +33605,7 @@
       <c r="A2289">
         <v>57815</v>
       </c>
-      <c r="B2289">
+      <c r="B2289" s="9">
         <v>0.63</v>
       </c>
       <c r="C2289" t="s">
@@ -33616,7 +33616,7 @@
       <c r="A2290">
         <v>57815</v>
       </c>
-      <c r="B2290">
+      <c r="B2290" s="9">
         <v>0.25700000000000001</v>
       </c>
       <c r="C2290" t="s">
@@ -33627,7 +33627,7 @@
       <c r="A2291">
         <v>57815</v>
       </c>
-      <c r="B2291">
+      <c r="B2291" s="9">
         <v>0.19600000000000001</v>
       </c>
       <c r="C2291" t="s">
@@ -33638,7 +33638,7 @@
       <c r="A2292">
         <v>57815</v>
       </c>
-      <c r="B2292">
+      <c r="B2292" s="9">
         <v>0.111</v>
       </c>
       <c r="C2292" t="s">
@@ -33649,7 +33649,7 @@
       <c r="A2293">
         <v>57815</v>
       </c>
-      <c r="B2293">
+      <c r="B2293" s="9">
         <v>0.436</v>
       </c>
       <c r="C2293" t="s">
@@ -34276,7 +34276,7 @@
       <c r="A2350">
         <v>58651</v>
       </c>
-      <c r="B2350">
+      <c r="B2350" s="9">
         <v>0.12859999999999999</v>
       </c>
       <c r="C2350" t="s">
@@ -34287,7 +34287,7 @@
       <c r="A2351">
         <v>58651</v>
       </c>
-      <c r="B2351">
+      <c r="B2351" s="12">
         <v>45995</v>
       </c>
       <c r="C2351" t="s">
@@ -34298,7 +34298,7 @@
       <c r="A2352">
         <v>58651</v>
       </c>
-      <c r="B2352">
+      <c r="B2352" s="11">
         <v>43525</v>
       </c>
       <c r="C2352" t="s">
@@ -34309,7 +34309,7 @@
       <c r="A2353">
         <v>58651</v>
       </c>
-      <c r="B2353">
+      <c r="B2353" s="12">
         <v>45748</v>
       </c>
       <c r="C2353" t="s">
@@ -34320,7 +34320,7 @@
       <c r="A2354">
         <v>58651</v>
       </c>
-      <c r="B2354">
+      <c r="B2354" s="11">
         <v>12785</v>
       </c>
       <c r="C2354" t="s">
@@ -34331,7 +34331,7 @@
       <c r="A2355">
         <v>58651</v>
       </c>
-      <c r="B2355">
+      <c r="B2355" s="12">
         <v>45902</v>
       </c>
       <c r="C2355" t="s">
@@ -34342,7 +34342,7 @@
       <c r="A2356">
         <v>58651</v>
       </c>
-      <c r="B2356">
+      <c r="B2356" s="12">
         <v>45689</v>
       </c>
       <c r="C2356" t="s">
@@ -34353,7 +34353,7 @@
       <c r="A2357">
         <v>58651</v>
       </c>
-      <c r="B2357">
+      <c r="B2357" s="12">
         <v>45962</v>
       </c>
       <c r="C2357" t="s">
@@ -34485,7 +34485,7 @@
       <c r="A2369">
         <v>58837</v>
       </c>
-      <c r="B2369">
+      <c r="B2369" s="8">
         <v>0.85</v>
       </c>
       <c r="C2369" t="s">
@@ -35739,7 +35739,7 @@
       <c r="A2483">
         <v>59196</v>
       </c>
-      <c r="B2483">
+      <c r="B2483" s="11">
         <v>44958</v>
       </c>
       <c r="C2483" t="s">
@@ -35871,7 +35871,7 @@
       <c r="A2495">
         <v>59228</v>
       </c>
-      <c r="B2495">
+      <c r="B2495" s="8">
         <v>0.8</v>
       </c>
       <c r="C2495" t="s">
@@ -35893,7 +35893,7 @@
       <c r="A2497">
         <v>59228</v>
       </c>
-      <c r="B2497">
+      <c r="B2497" s="8">
         <v>0.64</v>
       </c>
       <c r="C2497" t="s">
@@ -36080,7 +36080,7 @@
       <c r="A2514">
         <v>58036</v>
       </c>
-      <c r="B2514">
+      <c r="B2514" s="9">
         <v>0.997</v>
       </c>
       <c r="C2514" t="s">

</xml_diff>